<commit_message>
implemented choropleth map updates
</commit_message>
<xml_diff>
--- a/Server/TotalGHGEmissions.xlsx
+++ b/Server/TotalGHGEmissions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsancho\Documents\CURSOS\2021-2\Proyectos\Proyecto final\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres Aguilar Moya\Desktop\Visualizacion-PRY2-Global-Watch\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CC204E-0FAC-4601-AB3C-CFE0D09EFE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7020"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +28,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="4 total-ghg-emissions-excluding-lufc" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="4 total-ghg-emissions-excluding-lufc" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="C:\Users\lsancho\Documents\CURSOS\2021-2\Proyectos\Proyecto final\Datos\4 total-ghg-emissions-excluding-lufc.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -1211,7 +1212,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1261,7 +1262,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4 total-ghg-emissions-excluding-lufc" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="4 total-ghg-emissions-excluding-lufc" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1526,14 +1527,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>

</xml_diff>